<commit_message>
Set up array test
</commit_message>
<xml_diff>
--- a/Demo/Demo Sheet.xlsx
+++ b/Demo/Demo Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utiglobal-my.sharepoint.com/personal/ascinta_utiglobal_com/Documents/Documents/Excel Processor/Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{4B5143BC-719F-40C1-BEEF-834F15D291B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A2F5A6C-9DF1-4030-B1C6-1ABB1C763722}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{4B5143BC-719F-40C1-BEEF-834F15D291B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CB7CCE0-57C7-49EC-8B94-B5F1A8962B5E}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11235" xr2:uid="{D5A5015D-0334-49D1-8F43-91248DADCFE0}"/>
+    <workbookView xWindow="5190" yWindow="255" windowWidth="21600" windowHeight="10830" activeTab="1" xr2:uid="{D5A5015D-0334-49D1-8F43-91248DADCFE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,6 +119,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB82458-28DD-404D-9F90-8A887AA7F001}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -479,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FF2B10-7F9B-4390-89A1-48B71A2350BF}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,11 +549,11 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:C5" si="0">SUM(B3:B4)</f>
+        <f>SUM(B3:B4)</f>
         <v>5</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B5:C5" si="0">SUM(C3:C4)</f>
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pull information and set up config excel file
</commit_message>
<xml_diff>
--- a/Demo/Demo Sheet.xlsx
+++ b/Demo/Demo Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utiglobal-my.sharepoint.com/personal/ascinta_utiglobal_com/Documents/Documents/Excel Processor/Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{4B5143BC-719F-40C1-BEEF-834F15D291B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CB7CCE0-57C7-49EC-8B94-B5F1A8962B5E}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{4B5143BC-719F-40C1-BEEF-834F15D291B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4E58939-02D9-491B-B33E-9E537318A499}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="255" windowWidth="21600" windowHeight="10830" activeTab="1" xr2:uid="{D5A5015D-0334-49D1-8F43-91248DADCFE0}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{D5A5015D-0334-49D1-8F43-91248DADCFE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Demo information</t>
   </si>
@@ -48,18 +48,9 @@
     <t>Column B Header Text</t>
   </si>
   <si>
-    <t>Column C Header Text</t>
-  </si>
-  <si>
     <t>Junk A2 Text</t>
   </si>
   <si>
-    <t>Junk C3 text</t>
-  </si>
-  <si>
-    <t>Junk B2 text</t>
-  </si>
-  <si>
     <t>Dummy Sheet</t>
   </si>
   <si>
@@ -67,6 +58,36 @@
   </si>
   <si>
     <t>stuff</t>
+  </si>
+  <si>
+    <t>Device Name 1</t>
+  </si>
+  <si>
+    <t>CAM1</t>
+  </si>
+  <si>
+    <t>CAM2</t>
+  </si>
+  <si>
+    <t>CAM3</t>
+  </si>
+  <si>
+    <t>GSS1</t>
+  </si>
+  <si>
+    <t>KEY1</t>
+  </si>
+  <si>
+    <t>KEY2</t>
+  </si>
+  <si>
+    <t>INP1</t>
+  </si>
+  <si>
+    <t>INP2</t>
+  </si>
+  <si>
+    <t>CAM4</t>
   </si>
 </sst>
 </file>
@@ -460,18 +481,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -481,80 +502,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FF2B10-7F9B-4390-89A1-48B71A2350BF}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <f>2</f>
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <f>3</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>2</f>
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <f>3</f>
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <f>4</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f>SUM(A3:A4)</f>
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <f>SUM(B3:B4)</f>
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ref="B5:C5" si="0">SUM(C3:C4)</f>
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>